<commit_message>
MOD: Se actualiza hoja de excel pues había un error en el ordenamiento
</commit_message>
<xml_diff>
--- a/material/IntroProg/Notas/ResultadosParcial2/NotasParcial2-IntroProg2020-c.xlsx
+++ b/material/IntroProg/Notas/ResultadosParcial2/NotasParcial2-IntroProg2020-c.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85D78AC8-03D8-436A-A81E-D54E25C25AA5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A7340BD-2456-45F0-A73A-02F297CE9828}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -12,9 +12,9 @@
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'report name'!$B$2:$AI$32</definedName>
-    <definedName name="_xlchart.v1.0" hidden="1">'report name'!$T$3:$T$31</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">'report name'!$AI$3:$AI$29</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'report name'!$A$2:$AI$32</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">'report name'!$AI$3:$AI$29</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">'report name'!$T$3:$T$31</definedName>
     <definedName name="JR_PAGE_ANCHOR_0_1">'report name'!$B$1</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
@@ -44,7 +44,7 @@
     Estimada por mi, según lo que he observado de cada uno de ustedes. Es solo informativo</t>
       </text>
     </comment>
-    <comment ref="H28" authorId="1" shapeId="0" xr:uid="{F6E07B59-F3D8-46A6-ABBC-852B4845A740}">
+    <comment ref="H29" authorId="1" shapeId="0" xr:uid="{F6E07B59-F3D8-46A6-ABBC-852B4845A740}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -1007,7 +1007,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1192,26 +1192,41 @@
     <xf numFmtId="16" fontId="1" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1555,7 +1570,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.0</cx:f>
+        <cx:f>_xlchart.v1.1</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -1610,7 +1625,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.1</cx:f>
+        <cx:f>_xlchart.v1.0</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -3370,7 +3385,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="1181100" y="11266488"/>
+              <a:off x="3192780" y="11441748"/>
               <a:ext cx="0" cy="2633662"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -3484,7 +3499,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="2316480" y="11515453"/>
+              <a:off x="4328160" y="11690713"/>
               <a:ext cx="4749437" cy="2790553"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -3818,7 +3833,7 @@
   <threadedComment ref="Y2" dT="2020-03-25T21:03:18.32" personId="{00000000-0000-0000-0000-000000000000}" id="{2F1E3C2C-656A-409F-9056-E8FD594B3BFC}">
     <text>Estimada por mi, según lo que he observado de cada uno de ustedes. Es solo informativo</text>
   </threadedComment>
-  <threadedComment ref="H28" dT="2020-03-04T16:40:54.52" personId="{00000000-0000-0000-0000-000000000000}" id="{F6E07B59-F3D8-46A6-ABBC-852B4845A740}">
+  <threadedComment ref="H29" dT="2020-03-04T16:40:54.52" personId="{00000000-0000-0000-0000-000000000000}" id="{F6E07B59-F3D8-46A6-ABBC-852B4845A740}">
     <text>Si vino pero lo perdió en 0</text>
   </threadedComment>
 </ThreadedComments>
@@ -3835,7 +3850,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="X3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AC33" sqref="AC33"/>
+      <selection pane="bottomRight" sqref="A1:X1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8"/>
@@ -3995,7 +4010,7 @@
     </row>
     <row r="3" spans="1:71" s="34" customFormat="1" ht="19.95" customHeight="1">
       <c r="A3" s="54" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="B3" s="32" t="s">
         <v>130</v>
@@ -4019,7 +4034,7 @@
         <v>3.75</v>
       </c>
       <c r="I3" s="15">
-        <f t="shared" ref="I3:I32" si="0">(C3+D3+F3+H3)/4</f>
+        <f>(C3+D3+F3+H3)/4</f>
         <v>4.5125000000000002</v>
       </c>
       <c r="J3" s="15">
@@ -4053,12 +4068,12 @@
         <v>4</v>
       </c>
       <c r="T3" s="25">
-        <f t="shared" ref="T3:T32" si="1">Q3+R3</f>
+        <f>Q3+R3</f>
         <v>45</v>
       </c>
       <c r="U3" s="26"/>
       <c r="V3" s="26">
-        <f t="shared" ref="V3:V18" si="2">T3+U3</f>
+        <f>T3+U3</f>
         <v>45</v>
       </c>
       <c r="W3" s="26" t="s">
@@ -4095,11 +4110,11 @@
         <v>20</v>
       </c>
       <c r="AH3" s="57">
-        <f t="shared" ref="AH3:AH32" si="3">AE3+AF3+AG3</f>
+        <f>AE3+AF3+AG3</f>
         <v>50</v>
       </c>
       <c r="AI3" s="57">
-        <f t="shared" ref="AI3:AI18" si="4">AH3+J3</f>
+        <f>AH3+J3</f>
         <v>52</v>
       </c>
       <c r="AJ3" s="4"/>
@@ -4139,79 +4154,85 @@
     </row>
     <row r="4" spans="1:71" s="4" customFormat="1" ht="19.95" customHeight="1">
       <c r="A4" s="54" t="s">
-        <v>208</v>
+        <v>227</v>
       </c>
       <c r="B4" s="32" t="s">
-        <v>101</v>
+        <v>72</v>
       </c>
       <c r="C4" s="36">
         <v>5</v>
       </c>
-      <c r="D4" s="37">
-        <v>4.9000000000000004</v>
+      <c r="D4" s="74">
+        <v>5</v>
       </c>
       <c r="E4" s="38">
-        <v>4.9000000000000004</v>
+        <v>5</v>
       </c>
       <c r="F4" s="14">
         <v>5</v>
       </c>
-      <c r="G4" s="3"/>
+      <c r="G4" s="3" t="s">
+        <v>38</v>
+      </c>
       <c r="H4" s="37">
         <v>5</v>
       </c>
-      <c r="I4" s="15">
-        <f t="shared" si="0"/>
-        <v>4.9749999999999996</v>
-      </c>
-      <c r="J4" s="15">
+      <c r="I4" s="31">
+        <f>(C4+D4+F4+H4)/4</f>
+        <v>5</v>
+      </c>
+      <c r="J4" s="31">
         <v>2</v>
       </c>
       <c r="K4" s="37" t="s">
-        <v>102</v>
+        <v>39</v>
       </c>
       <c r="L4" s="37" t="s">
-        <v>34</v>
-      </c>
-      <c r="M4" s="16">
-        <v>7</v>
-      </c>
-      <c r="N4" s="24"/>
+        <v>39</v>
+      </c>
+      <c r="M4" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="N4" s="24" t="s">
+        <v>73</v>
+      </c>
       <c r="O4" s="25">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="P4" s="25">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="Q4" s="25">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="R4" s="25">
         <v>10</v>
       </c>
       <c r="S4" s="25">
+        <v>4</v>
+      </c>
+      <c r="T4" s="25">
+        <f>Q4+R4</f>
+        <v>48</v>
+      </c>
+      <c r="U4" s="26">
+        <v>1</v>
+      </c>
+      <c r="V4" s="26">
+        <f>T4+U4</f>
+        <v>49</v>
+      </c>
+      <c r="W4" s="26">
         <v>7</v>
       </c>
-      <c r="T4" s="25">
-        <f t="shared" si="1"/>
-        <v>50</v>
-      </c>
-      <c r="U4" s="26"/>
-      <c r="V4" s="26">
-        <f t="shared" si="2"/>
-        <v>50</v>
-      </c>
-      <c r="W4" s="26">
-        <v>10</v>
-      </c>
       <c r="X4" s="57" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="Y4" s="57">
-        <v>4</v>
+        <v>4.3</v>
       </c>
       <c r="Z4" s="57">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AA4" s="57" t="s">
         <v>148</v>
@@ -4235,11 +4256,11 @@
         <v>20</v>
       </c>
       <c r="AH4" s="57">
-        <f t="shared" si="3"/>
+        <f>AE4+AF4+AG4</f>
         <v>50</v>
       </c>
       <c r="AI4" s="57">
-        <f t="shared" si="4"/>
+        <f>AH4+J4</f>
         <v>52</v>
       </c>
       <c r="BR4" s="3"/>
@@ -4247,85 +4268,79 @@
     </row>
     <row r="5" spans="1:71" s="34" customFormat="1" ht="19.95" customHeight="1">
       <c r="A5" s="54" t="s">
-        <v>209</v>
+        <v>220</v>
       </c>
       <c r="B5" s="32" t="s">
-        <v>72</v>
+        <v>101</v>
       </c>
       <c r="C5" s="36">
         <v>5</v>
       </c>
-      <c r="D5" s="69">
-        <v>5</v>
+      <c r="D5" s="37">
+        <v>4.9000000000000004</v>
       </c>
       <c r="E5" s="38">
-        <v>5</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="F5" s="14">
         <v>5</v>
       </c>
-      <c r="G5" s="3" t="s">
-        <v>38</v>
-      </c>
+      <c r="G5" s="3"/>
       <c r="H5" s="37">
         <v>5</v>
       </c>
-      <c r="I5" s="31">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="J5" s="31">
+      <c r="I5" s="15">
+        <f>(C5+D5+F5+H5)/4</f>
+        <v>4.9749999999999996</v>
+      </c>
+      <c r="J5" s="15">
         <v>2</v>
       </c>
       <c r="K5" s="37" t="s">
-        <v>39</v>
+        <v>102</v>
       </c>
       <c r="L5" s="37" t="s">
-        <v>39</v>
-      </c>
-      <c r="M5" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="M5" s="16">
+        <v>7</v>
+      </c>
+      <c r="N5" s="24"/>
+      <c r="O5" s="25">
+        <v>4</v>
+      </c>
+      <c r="P5" s="25">
+        <v>31</v>
+      </c>
+      <c r="Q5" s="25">
         <v>40</v>
-      </c>
-      <c r="N5" s="24" t="s">
-        <v>73</v>
-      </c>
-      <c r="O5" s="25">
-        <v>5</v>
-      </c>
-      <c r="P5" s="25">
-        <v>18</v>
-      </c>
-      <c r="Q5" s="25">
-        <v>38</v>
       </c>
       <c r="R5" s="25">
         <v>10</v>
       </c>
       <c r="S5" s="25">
+        <v>7</v>
+      </c>
+      <c r="T5" s="25">
+        <f>Q5+R5</f>
+        <v>50</v>
+      </c>
+      <c r="U5" s="26"/>
+      <c r="V5" s="26">
+        <f>T5+U5</f>
+        <v>50</v>
+      </c>
+      <c r="W5" s="26">
+        <v>10</v>
+      </c>
+      <c r="X5" s="57" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y5" s="57">
         <v>4</v>
       </c>
-      <c r="T5" s="25">
-        <f t="shared" si="1"/>
-        <v>48</v>
-      </c>
-      <c r="U5" s="26">
+      <c r="Z5" s="57">
         <v>1</v>
-      </c>
-      <c r="V5" s="26">
-        <f t="shared" si="2"/>
-        <v>49</v>
-      </c>
-      <c r="W5" s="26">
-        <v>7</v>
-      </c>
-      <c r="X5" s="57" t="s">
-        <v>42</v>
-      </c>
-      <c r="Y5" s="57">
-        <v>4.3</v>
-      </c>
-      <c r="Z5" s="57">
-        <v>2</v>
       </c>
       <c r="AA5" s="57" t="s">
         <v>148</v>
@@ -4349,11 +4364,11 @@
         <v>20</v>
       </c>
       <c r="AH5" s="57">
-        <f t="shared" si="3"/>
+        <f>AE5+AF5+AG5</f>
         <v>50</v>
       </c>
       <c r="AI5" s="57">
-        <f t="shared" si="4"/>
+        <f>AH5+J5</f>
         <v>52</v>
       </c>
       <c r="AJ5" s="4"/>
@@ -4393,100 +4408,94 @@
     </row>
     <row r="6" spans="1:71" s="4" customFormat="1" ht="32.4" customHeight="1">
       <c r="A6" s="54" t="s">
-        <v>210</v>
+        <v>229</v>
       </c>
       <c r="B6" s="32" t="s">
-        <v>105</v>
+        <v>66</v>
       </c>
       <c r="C6" s="11">
+        <v>5</v>
+      </c>
+      <c r="D6" s="12">
+        <v>4.8</v>
+      </c>
+      <c r="E6" s="13">
         <v>4.5</v>
       </c>
-      <c r="D6" s="12">
-        <v>4.8499999999999996</v>
-      </c>
-      <c r="E6" s="13">
-        <v>5</v>
-      </c>
       <c r="F6" s="14">
         <v>5</v>
       </c>
-      <c r="G6" s="3" t="s">
-        <v>83</v>
-      </c>
+      <c r="G6" s="3"/>
       <c r="H6" s="12">
         <v>5</v>
       </c>
       <c r="I6" s="15">
-        <f t="shared" si="0"/>
-        <v>4.8375000000000004</v>
+        <f>(C6+D6+F6+H6)/4</f>
+        <v>4.95</v>
       </c>
       <c r="J6" s="15">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K6" s="12" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="L6" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="M6" s="18" t="s">
-        <v>40</v>
+        <v>46</v>
+      </c>
+      <c r="M6" s="16">
+        <v>8</v>
       </c>
       <c r="N6" s="24" t="s">
-        <v>106</v>
+        <v>67</v>
       </c>
       <c r="O6" s="25">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="P6" s="25">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="Q6" s="25">
         <v>40</v>
       </c>
       <c r="R6" s="25">
+        <v>10</v>
+      </c>
+      <c r="S6" s="25"/>
+      <c r="T6" s="25">
+        <f>Q6+R6</f>
+        <v>50</v>
+      </c>
+      <c r="U6" s="26"/>
+      <c r="V6" s="26">
+        <f>T6+U6</f>
+        <v>50</v>
+      </c>
+      <c r="W6" s="26">
         <v>2</v>
       </c>
-      <c r="S6" s="25">
-        <v>0</v>
-      </c>
-      <c r="T6" s="25">
-        <f t="shared" si="1"/>
-        <v>42</v>
-      </c>
-      <c r="U6" s="26">
-        <v>1</v>
-      </c>
-      <c r="V6" s="26">
-        <f t="shared" si="2"/>
-        <v>43</v>
-      </c>
-      <c r="W6" s="26">
-        <v>10</v>
-      </c>
       <c r="X6" s="57" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="Y6" s="57">
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="Z6" s="57">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="AA6" s="57" t="s">
+        <v>160</v>
+      </c>
+      <c r="AB6" s="57" t="s">
         <v>151</v>
       </c>
-      <c r="AB6" s="61" t="s">
-        <v>166</v>
-      </c>
-      <c r="AC6" s="58" t="s">
-        <v>205</v>
+      <c r="AC6" s="57" t="s">
+        <v>151</v>
       </c>
       <c r="AD6" s="58" t="s">
         <v>150</v>
       </c>
       <c r="AE6" s="57">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="AF6" s="57">
         <v>20</v>
@@ -4495,11 +4504,11 @@
         <v>20</v>
       </c>
       <c r="AH6" s="57">
-        <f t="shared" si="3"/>
-        <v>50</v>
+        <f>AE6+AF6+AG6</f>
+        <v>48</v>
       </c>
       <c r="AI6" s="57">
-        <f t="shared" si="4"/>
+        <f>AH6+J6</f>
         <v>50</v>
       </c>
       <c r="BR6" s="3"/>
@@ -4507,7 +4516,7 @@
     </row>
     <row r="7" spans="1:71" s="19" customFormat="1" ht="19.95" customHeight="1">
       <c r="A7" s="54" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="B7" s="32" t="s">
         <v>117</v>
@@ -4531,7 +4540,7 @@
         <v>0</v>
       </c>
       <c r="I7" s="15">
-        <f t="shared" si="0"/>
+        <f>(C7+D7+F7+H7)/4</f>
         <v>3.75</v>
       </c>
       <c r="J7" s="15">
@@ -4563,12 +4572,12 @@
         <v>0</v>
       </c>
       <c r="T7" s="25">
-        <f t="shared" si="1"/>
+        <f>Q7+R7</f>
         <v>50</v>
       </c>
       <c r="U7" s="26"/>
       <c r="V7" s="26">
-        <f t="shared" si="2"/>
+        <f>T7+U7</f>
         <v>50</v>
       </c>
       <c r="W7" s="26">
@@ -4605,11 +4614,11 @@
         <v>18</v>
       </c>
       <c r="AH7" s="57">
-        <f t="shared" si="3"/>
+        <f>AE7+AF7+AG7</f>
         <v>48</v>
       </c>
       <c r="AI7" s="57">
-        <f t="shared" si="4"/>
+        <f>AH7+J7</f>
         <v>50</v>
       </c>
       <c r="AJ7" s="4"/>
@@ -4649,94 +4658,100 @@
     </row>
     <row r="8" spans="1:71" s="4" customFormat="1" ht="31.8" customHeight="1">
       <c r="A8" s="54" t="s">
-        <v>212</v>
+        <v>218</v>
       </c>
       <c r="B8" s="32" t="s">
-        <v>66</v>
+        <v>105</v>
       </c>
       <c r="C8" s="11">
-        <v>5</v>
+        <v>4.5</v>
       </c>
       <c r="D8" s="12">
-        <v>4.8</v>
+        <v>4.8499999999999996</v>
       </c>
       <c r="E8" s="13">
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="F8" s="14">
         <v>5</v>
       </c>
-      <c r="G8" s="3"/>
+      <c r="G8" s="3" t="s">
+        <v>83</v>
+      </c>
       <c r="H8" s="12">
         <v>5</v>
       </c>
       <c r="I8" s="15">
-        <f t="shared" si="0"/>
-        <v>4.95</v>
+        <f>(C8+D8+F8+H8)/4</f>
+        <v>4.8375000000000004</v>
       </c>
       <c r="J8" s="15">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K8" s="12" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="L8" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="M8" s="16">
-        <v>8</v>
+        <v>39</v>
+      </c>
+      <c r="M8" s="18" t="s">
+        <v>40</v>
       </c>
       <c r="N8" s="24" t="s">
-        <v>67</v>
+        <v>106</v>
       </c>
       <c r="O8" s="25">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="P8" s="25">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="Q8" s="25">
         <v>40</v>
       </c>
       <c r="R8" s="25">
+        <v>2</v>
+      </c>
+      <c r="S8" s="25">
+        <v>0</v>
+      </c>
+      <c r="T8" s="25">
+        <f>Q8+R8</f>
+        <v>42</v>
+      </c>
+      <c r="U8" s="26">
+        <v>1</v>
+      </c>
+      <c r="V8" s="26">
+        <f>T8+U8</f>
+        <v>43</v>
+      </c>
+      <c r="W8" s="26">
         <v>10</v>
       </c>
-      <c r="S8" s="25"/>
-      <c r="T8" s="25">
-        <f t="shared" si="1"/>
-        <v>50</v>
-      </c>
-      <c r="U8" s="26"/>
-      <c r="V8" s="26">
-        <f t="shared" si="2"/>
-        <v>50</v>
-      </c>
-      <c r="W8" s="26">
-        <v>2</v>
-      </c>
       <c r="X8" s="57" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="Y8" s="57">
-        <v>3.5</v>
+        <v>4.5</v>
       </c>
       <c r="Z8" s="57">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="AA8" s="57" t="s">
-        <v>160</v>
-      </c>
-      <c r="AB8" s="57" t="s">
         <v>151</v>
       </c>
-      <c r="AC8" s="57" t="s">
-        <v>151</v>
+      <c r="AB8" s="61" t="s">
+        <v>166</v>
+      </c>
+      <c r="AC8" s="58" t="s">
+        <v>205</v>
       </c>
       <c r="AD8" s="58" t="s">
         <v>150</v>
       </c>
       <c r="AE8" s="57">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="AF8" s="57">
         <v>20</v>
@@ -4745,11 +4760,11 @@
         <v>20</v>
       </c>
       <c r="AH8" s="57">
-        <f t="shared" si="3"/>
-        <v>48</v>
+        <f>AE8+AF8+AG8</f>
+        <v>50</v>
       </c>
       <c r="AI8" s="57">
-        <f t="shared" si="4"/>
+        <f>AH8+J8</f>
         <v>50</v>
       </c>
       <c r="BR8" s="3"/>
@@ -4757,7 +4772,7 @@
     </row>
     <row r="9" spans="1:71" s="4" customFormat="1" ht="19.95" customHeight="1">
       <c r="A9" s="54" t="s">
-        <v>213</v>
+        <v>236</v>
       </c>
       <c r="B9" s="40" t="s">
         <v>31</v>
@@ -4781,7 +4796,7 @@
         <v>5</v>
       </c>
       <c r="I9" s="42">
-        <f t="shared" si="0"/>
+        <f>(C9+D9+F9+H9)/4</f>
         <v>5</v>
       </c>
       <c r="J9" s="42">
@@ -4815,11 +4830,11 @@
         <v>0</v>
       </c>
       <c r="T9" s="44">
-        <f t="shared" si="1"/>
+        <f>Q9+R9</f>
         <v>50</v>
       </c>
       <c r="V9" s="4">
-        <f t="shared" si="2"/>
+        <f>T9+U9</f>
         <v>50</v>
       </c>
       <c r="W9" s="26">
@@ -4856,11 +4871,11 @@
         <v>18</v>
       </c>
       <c r="AH9" s="57">
-        <f t="shared" si="3"/>
+        <f>AE9+AF9+AG9</f>
         <v>46</v>
       </c>
       <c r="AI9" s="57">
-        <f t="shared" si="4"/>
+        <f>AH9+J9</f>
         <v>48</v>
       </c>
       <c r="BR9" s="3"/>
@@ -4868,7 +4883,7 @@
     </row>
     <row r="10" spans="1:71" s="4" customFormat="1" ht="19.95" customHeight="1">
       <c r="A10" s="54" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="B10" s="32" t="s">
         <v>107</v>
@@ -4890,7 +4905,7 @@
         <v>4.5</v>
       </c>
       <c r="I10" s="15">
-        <f t="shared" si="0"/>
+        <f>(C10+D10+F10+H10)/4</f>
         <v>4.75</v>
       </c>
       <c r="J10" s="15">
@@ -4924,12 +4939,12 @@
         <v>-2</v>
       </c>
       <c r="T10" s="25">
-        <f t="shared" si="1"/>
+        <f>Q10+R10</f>
         <v>48</v>
       </c>
       <c r="U10" s="26"/>
       <c r="V10" s="26">
-        <f t="shared" si="2"/>
+        <f>T10+U10</f>
         <v>48</v>
       </c>
       <c r="W10" s="26"/>
@@ -4964,11 +4979,11 @@
         <v>18</v>
       </c>
       <c r="AH10" s="57">
-        <f t="shared" si="3"/>
+        <f>AE10+AF10+AG10</f>
         <v>46</v>
       </c>
       <c r="AI10" s="57">
-        <f t="shared" si="4"/>
+        <f>AH10+J10</f>
         <v>46</v>
       </c>
       <c r="BR10" s="3"/>
@@ -4976,33 +4991,35 @@
     </row>
     <row r="11" spans="1:71" s="4" customFormat="1" ht="19.95" customHeight="1">
       <c r="A11" s="54" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="B11" s="32" t="s">
-        <v>125</v>
+        <v>88</v>
       </c>
       <c r="C11" s="11">
         <v>5</v>
       </c>
       <c r="D11" s="12">
-        <v>2.5</v>
+        <v>4.8</v>
       </c>
       <c r="E11" s="13">
         <v>2</v>
       </c>
-      <c r="F11" s="21">
-        <v>5</v>
-      </c>
-      <c r="G11" s="3"/>
+      <c r="F11" s="14">
+        <v>5</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>89</v>
+      </c>
       <c r="H11" s="12">
-        <v>5</v>
+        <v>3.75</v>
       </c>
       <c r="I11" s="15">
-        <f t="shared" si="0"/>
-        <v>4.375</v>
+        <f>(C11+D11+F11+H11)/4</f>
+        <v>4.6375000000000002</v>
       </c>
       <c r="J11" s="15">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K11" s="12" t="s">
         <v>90</v>
@@ -5010,73 +5027,75 @@
       <c r="L11" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="M11" s="33">
+      <c r="M11" s="20">
         <v>4</v>
       </c>
-      <c r="N11" s="24"/>
+      <c r="N11" s="24" t="s">
+        <v>92</v>
+      </c>
       <c r="O11" s="25">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="P11" s="25">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="Q11" s="25">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="R11" s="25">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="S11" s="25">
         <v>0</v>
       </c>
       <c r="T11" s="25">
-        <f t="shared" si="1"/>
-        <v>41</v>
+        <f>Q11+R11</f>
+        <v>48</v>
       </c>
       <c r="U11" s="26"/>
       <c r="V11" s="26">
-        <f t="shared" si="2"/>
-        <v>41</v>
+        <f>T11+U11</f>
+        <v>48</v>
       </c>
       <c r="W11" s="26">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="X11" s="57" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="Y11" s="57">
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="Z11" s="57">
-        <v>12</v>
-      </c>
-      <c r="AA11" s="57">
-        <v>5</v>
-      </c>
-      <c r="AB11" s="57">
+        <v>29</v>
+      </c>
+      <c r="AA11" s="57" t="s">
+        <v>164</v>
+      </c>
+      <c r="AB11" s="57" t="s">
+        <v>153</v>
+      </c>
+      <c r="AC11" s="57" t="s">
+        <v>204</v>
+      </c>
+      <c r="AD11" s="58" t="s">
+        <v>165</v>
+      </c>
+      <c r="AE11" s="57">
         <v>9</v>
       </c>
-      <c r="AC11" s="57">
-        <v>9</v>
-      </c>
-      <c r="AD11" s="58" t="s">
-        <v>161</v>
-      </c>
-      <c r="AE11" s="57">
-        <v>5</v>
-      </c>
       <c r="AF11" s="57">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="AG11" s="57">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="AH11" s="57">
-        <f t="shared" si="3"/>
-        <v>45</v>
+        <f>AE11+AF11+AG11</f>
+        <v>43</v>
       </c>
       <c r="AI11" s="57">
-        <f t="shared" si="4"/>
+        <f>AH11+J11</f>
         <v>45</v>
       </c>
       <c r="BR11" s="3"/>
@@ -5084,35 +5103,33 @@
     </row>
     <row r="12" spans="1:71" s="4" customFormat="1" ht="77.400000000000006" customHeight="1">
       <c r="A12" s="54" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="B12" s="32" t="s">
-        <v>88</v>
+        <v>125</v>
       </c>
       <c r="C12" s="36">
         <v>5</v>
       </c>
       <c r="D12" s="37">
-        <v>4.8</v>
+        <v>2.5</v>
       </c>
       <c r="E12" s="38">
         <v>2</v>
       </c>
-      <c r="F12" s="14">
-        <v>5</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>89</v>
-      </c>
+      <c r="F12" s="21">
+        <v>5</v>
+      </c>
+      <c r="G12" s="3"/>
       <c r="H12" s="37">
-        <v>3.75</v>
+        <v>5</v>
       </c>
       <c r="I12" s="15">
-        <f t="shared" si="0"/>
-        <v>4.6375000000000002</v>
+        <f>(C12+D12+F12+H12)/4</f>
+        <v>4.375</v>
       </c>
       <c r="J12" s="15">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K12" s="37" t="s">
         <v>90</v>
@@ -5120,75 +5137,73 @@
       <c r="L12" s="37" t="s">
         <v>91</v>
       </c>
-      <c r="M12" s="20">
+      <c r="M12" s="33">
         <v>4</v>
       </c>
-      <c r="N12" s="24" t="s">
-        <v>92</v>
-      </c>
+      <c r="N12" s="24"/>
       <c r="O12" s="25">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="P12" s="25">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="Q12" s="25">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="R12" s="25">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="S12" s="25">
         <v>0</v>
       </c>
       <c r="T12" s="25">
-        <f t="shared" si="1"/>
-        <v>48</v>
+        <f>Q12+R12</f>
+        <v>41</v>
       </c>
       <c r="U12" s="26"/>
       <c r="V12" s="26">
-        <f t="shared" si="2"/>
-        <v>48</v>
+        <f>T12+U12</f>
+        <v>41</v>
       </c>
       <c r="W12" s="26">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="X12" s="57" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="Y12" s="57">
-        <v>5</v>
+        <v>4.5</v>
       </c>
       <c r="Z12" s="57">
-        <v>29</v>
-      </c>
-      <c r="AA12" s="57" t="s">
-        <v>164</v>
-      </c>
-      <c r="AB12" s="57" t="s">
-        <v>153</v>
-      </c>
-      <c r="AC12" s="57" t="s">
-        <v>204</v>
+        <v>12</v>
+      </c>
+      <c r="AA12" s="57">
+        <v>5</v>
+      </c>
+      <c r="AB12" s="57">
+        <v>9</v>
+      </c>
+      <c r="AC12" s="57">
+        <v>9</v>
       </c>
       <c r="AD12" s="58" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="AE12" s="57">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="AF12" s="57">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="AG12" s="57">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="AH12" s="57">
-        <f t="shared" si="3"/>
-        <v>43</v>
+        <f>AE12+AF12+AG12</f>
+        <v>45</v>
       </c>
       <c r="AI12" s="57">
-        <f t="shared" si="4"/>
+        <f>AH12+J12</f>
         <v>45</v>
       </c>
       <c r="BR12" s="3"/>
@@ -5196,7 +5211,7 @@
     </row>
     <row r="13" spans="1:71" s="4" customFormat="1" ht="27" customHeight="1">
       <c r="A13" s="54" t="s">
-        <v>217</v>
+        <v>231</v>
       </c>
       <c r="B13" s="32" t="s">
         <v>60</v>
@@ -5220,7 +5235,7 @@
         <v>1.25</v>
       </c>
       <c r="I13" s="15">
-        <f t="shared" si="0"/>
+        <f>(C13+D13+F13+H13)/4</f>
         <v>1.5625</v>
       </c>
       <c r="J13" s="31">
@@ -5254,12 +5269,12 @@
         <v>1</v>
       </c>
       <c r="T13" s="25">
-        <f t="shared" si="1"/>
+        <f>Q13+R13</f>
         <v>47</v>
       </c>
       <c r="U13" s="26"/>
       <c r="V13" s="26">
-        <f t="shared" si="2"/>
+        <f>T13+U13</f>
         <v>47</v>
       </c>
       <c r="W13" s="26">
@@ -5296,11 +5311,11 @@
         <v>19</v>
       </c>
       <c r="AH13" s="57">
-        <f t="shared" si="3"/>
+        <f>AE13+AF13+AG13</f>
         <v>43</v>
       </c>
       <c r="AI13" s="57">
-        <f t="shared" si="4"/>
+        <f>AH13+J13</f>
         <v>45</v>
       </c>
       <c r="BR13" s="3"/>
@@ -5308,7 +5323,7 @@
     </row>
     <row r="14" spans="1:71" s="4" customFormat="1" ht="19.95" customHeight="1">
       <c r="A14" s="54" t="s">
-        <v>218</v>
+        <v>207</v>
       </c>
       <c r="B14" s="32" t="s">
         <v>140</v>
@@ -5330,7 +5345,7 @@
         <v>3.75</v>
       </c>
       <c r="I14" s="15">
-        <f t="shared" si="0"/>
+        <f>(C14+D14+F14+H14)/4</f>
         <v>4.6124999999999998</v>
       </c>
       <c r="J14" s="15">
@@ -5364,12 +5379,12 @@
         <v>2</v>
       </c>
       <c r="T14" s="25">
-        <f t="shared" si="1"/>
+        <f>Q14+R14</f>
         <v>46</v>
       </c>
       <c r="U14" s="26"/>
       <c r="V14" s="26">
-        <f t="shared" si="2"/>
+        <f>T14+U14</f>
         <v>46</v>
       </c>
       <c r="W14" s="26">
@@ -5402,11 +5417,11 @@
         <v>19</v>
       </c>
       <c r="AH14" s="57">
-        <f t="shared" si="3"/>
+        <f>AE14+AF14+AG14</f>
         <v>42</v>
       </c>
       <c r="AI14" s="57">
-        <f t="shared" si="4"/>
+        <f>AH14+J14</f>
         <v>44</v>
       </c>
       <c r="BR14" s="3"/>
@@ -5414,7 +5429,7 @@
     </row>
     <row r="15" spans="1:71" s="4" customFormat="1" ht="19.95" customHeight="1">
       <c r="A15" s="54" t="s">
-        <v>219</v>
+        <v>225</v>
       </c>
       <c r="B15" s="32" t="s">
         <v>79</v>
@@ -5436,7 +5451,7 @@
         <v>3.75</v>
       </c>
       <c r="I15" s="15">
-        <f t="shared" si="0"/>
+        <f>(C15+D15+F15+H15)/4</f>
         <v>4.1375000000000002</v>
       </c>
       <c r="J15" s="15">
@@ -5468,12 +5483,12 @@
         <v>2</v>
       </c>
       <c r="T15" s="25">
-        <f t="shared" si="1"/>
+        <f>Q15+R15</f>
         <v>41</v>
       </c>
       <c r="U15" s="26"/>
       <c r="V15" s="26">
-        <f t="shared" si="2"/>
+        <f>T15+U15</f>
         <v>41</v>
       </c>
       <c r="W15" s="26">
@@ -5508,11 +5523,11 @@
         <v>16</v>
       </c>
       <c r="AH15" s="57">
-        <f t="shared" si="3"/>
+        <f>AE15+AF15+AG15</f>
         <v>40</v>
       </c>
       <c r="AI15" s="57">
-        <f t="shared" si="4"/>
+        <f>AH15+J15</f>
         <v>42</v>
       </c>
       <c r="BR15" s="3"/>
@@ -5520,7 +5535,7 @@
     </row>
     <row r="16" spans="1:71" s="4" customFormat="1" ht="34.200000000000003" customHeight="1">
       <c r="A16" s="54" t="s">
-        <v>220</v>
+        <v>230</v>
       </c>
       <c r="B16" s="32" t="s">
         <v>62</v>
@@ -5542,7 +5557,7 @@
         <v>3.75</v>
       </c>
       <c r="I16" s="15">
-        <f t="shared" si="0"/>
+        <f>(C16+D16+F16+H16)/4</f>
         <v>4.6500000000000004</v>
       </c>
       <c r="J16" s="15">
@@ -5576,14 +5591,14 @@
         <v>0</v>
       </c>
       <c r="T16" s="25">
-        <f t="shared" si="1"/>
+        <f>Q16+R16</f>
         <v>47</v>
       </c>
       <c r="U16" s="26">
         <v>1</v>
       </c>
       <c r="V16" s="26">
-        <f t="shared" si="2"/>
+        <f>T16+U16</f>
         <v>48</v>
       </c>
       <c r="W16" s="26">
@@ -5620,11 +5635,11 @@
         <v>15</v>
       </c>
       <c r="AH16" s="57">
-        <f t="shared" si="3"/>
+        <f>AE16+AF16+AG16</f>
         <v>33</v>
       </c>
       <c r="AI16" s="57">
-        <f t="shared" si="4"/>
+        <f>AH16+J16</f>
         <v>35</v>
       </c>
       <c r="BR16" s="3"/>
@@ -5632,7 +5647,7 @@
     </row>
     <row r="17" spans="1:71" s="4" customFormat="1" ht="19.95" customHeight="1">
       <c r="A17" s="54" t="s">
-        <v>221</v>
+        <v>228</v>
       </c>
       <c r="B17" s="32" t="s">
         <v>68</v>
@@ -5654,7 +5669,7 @@
         <v>3.75</v>
       </c>
       <c r="I17" s="15">
-        <f t="shared" si="0"/>
+        <f>(C17+D17+F17+H17)/4</f>
         <v>4.6875</v>
       </c>
       <c r="J17" s="15">
@@ -5688,12 +5703,12 @@
         <v>0</v>
       </c>
       <c r="T17" s="25">
-        <f t="shared" si="1"/>
+        <f>Q17+R17</f>
         <v>45</v>
       </c>
       <c r="U17" s="26"/>
       <c r="V17" s="26">
-        <f t="shared" si="2"/>
+        <f>T17+U17</f>
         <v>45</v>
       </c>
       <c r="W17" s="26">
@@ -5728,11 +5743,11 @@
         <v>10</v>
       </c>
       <c r="AH17" s="57">
-        <f t="shared" si="3"/>
+        <f>AE17+AF17+AG17</f>
         <v>33</v>
       </c>
       <c r="AI17" s="57">
-        <f t="shared" si="4"/>
+        <f>AH17+J17</f>
         <v>33</v>
       </c>
       <c r="BR17" s="3"/>
@@ -5740,7 +5755,7 @@
     </row>
     <row r="18" spans="1:71" s="4" customFormat="1" ht="19.95" customHeight="1">
       <c r="A18" s="54" t="s">
-        <v>222</v>
+        <v>235</v>
       </c>
       <c r="B18" s="32" t="s">
         <v>37</v>
@@ -5764,7 +5779,7 @@
         <v>3.5</v>
       </c>
       <c r="I18" s="15">
-        <f t="shared" si="0"/>
+        <f>(C18+D18+F18+H18)/4</f>
         <v>4</v>
       </c>
       <c r="J18" s="15">
@@ -5798,14 +5813,14 @@
         <v>0</v>
       </c>
       <c r="T18" s="25">
-        <f t="shared" si="1"/>
+        <f>Q18+R18</f>
         <v>46</v>
       </c>
       <c r="U18" s="26">
         <v>1</v>
       </c>
       <c r="V18" s="26">
-        <f t="shared" si="2"/>
+        <f>T18+U18</f>
         <v>47</v>
       </c>
       <c r="W18" s="26">
@@ -5840,11 +5855,11 @@
         <v>9</v>
       </c>
       <c r="AH18" s="57">
-        <f t="shared" si="3"/>
+        <f>AE18+AF18+AG18</f>
         <v>33</v>
       </c>
       <c r="AI18" s="57">
-        <f t="shared" si="4"/>
+        <f>AH18+J18</f>
         <v>33</v>
       </c>
       <c r="BR18" s="3"/>
@@ -5852,108 +5867,107 @@
     </row>
     <row r="19" spans="1:71" s="4" customFormat="1" ht="30.6" customHeight="1">
       <c r="A19" s="54" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="B19" s="32" t="s">
-        <v>49</v>
+        <v>109</v>
       </c>
       <c r="C19" s="11">
+        <v>4.5</v>
+      </c>
+      <c r="D19" s="12">
+        <v>4.8</v>
+      </c>
+      <c r="E19" s="13">
+        <v>4</v>
+      </c>
+      <c r="F19" s="14">
+        <v>5</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="H19" s="12">
         <v>3.5</v>
       </c>
-      <c r="D19" s="12">
-        <v>1.5</v>
-      </c>
-      <c r="E19" s="13">
-        <v>0</v>
-      </c>
-      <c r="F19" s="14">
-        <v>0</v>
-      </c>
-      <c r="G19" s="3"/>
-      <c r="H19" s="12">
-        <v>0</v>
-      </c>
       <c r="I19" s="15">
-        <f t="shared" si="0"/>
-        <v>1.25</v>
-      </c>
-      <c r="J19" s="15" t="s">
-        <v>50</v>
+        <f>(C19+D19+F19+H19)/4</f>
+        <v>4.45</v>
+      </c>
+      <c r="J19" s="15">
+        <v>2</v>
       </c>
       <c r="K19" s="12" t="s">
-        <v>51</v>
+        <v>111</v>
       </c>
       <c r="L19" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="M19" s="16" t="s">
-        <v>51</v>
+        <v>112</v>
+      </c>
+      <c r="M19" s="16">
+        <v>8</v>
       </c>
       <c r="N19" s="24" t="s">
-        <v>52</v>
+        <v>113</v>
       </c>
       <c r="O19" s="25">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="P19" s="25">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="Q19" s="25">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="R19" s="25">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="S19" s="25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T19" s="25">
-        <f t="shared" si="1"/>
-        <v>38</v>
-      </c>
-      <c r="U19" s="26" t="s">
-        <v>53</v>
-      </c>
+        <f>Q19+R19</f>
+        <v>40</v>
+      </c>
+      <c r="U19" s="26"/>
       <c r="V19" s="26">
-        <f>T19</f>
-        <v>38</v>
+        <f>T19+U19</f>
+        <v>40</v>
       </c>
       <c r="W19" s="26">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="X19" s="57" t="s">
-        <v>54</v>
+        <v>36</v>
       </c>
       <c r="Y19" s="57">
-        <v>2</v>
+        <v>4.5</v>
       </c>
       <c r="Z19" s="57">
-        <v>22</v>
-      </c>
-      <c r="AA19" s="57">
-        <v>1</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="AA19" s="57"/>
       <c r="AB19" s="57" t="s">
-        <v>168</v>
+        <v>190</v>
       </c>
       <c r="AC19" s="57" t="s">
-        <v>238</v>
+        <v>191</v>
       </c>
       <c r="AD19" s="58"/>
       <c r="AE19" s="57">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="AF19" s="57">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="AG19" s="57">
         <v>4</v>
       </c>
       <c r="AH19" s="57">
-        <f t="shared" si="3"/>
-        <v>25</v>
+        <f>AE19+AF19+AG19</f>
+        <v>23</v>
       </c>
       <c r="AI19" s="57">
+        <f>AH19+J19</f>
         <v>25</v>
       </c>
       <c r="BR19" s="3"/>
@@ -5961,7 +5975,7 @@
     </row>
     <row r="20" spans="1:71" s="35" customFormat="1" ht="19.95" customHeight="1">
       <c r="A20" s="54" t="s">
-        <v>224</v>
+        <v>209</v>
       </c>
       <c r="B20" s="32" t="s">
         <v>135</v>
@@ -5983,7 +5997,7 @@
         <v>3.75</v>
       </c>
       <c r="I20" s="15">
-        <f t="shared" si="0"/>
+        <f>(C20+D20+F20+H20)/4</f>
         <v>4.6875</v>
       </c>
       <c r="J20" s="15">
@@ -6013,12 +6027,12 @@
         <v>0</v>
       </c>
       <c r="T20" s="25">
-        <f t="shared" si="1"/>
+        <f>Q20+R20</f>
         <v>50</v>
       </c>
       <c r="U20" s="26"/>
       <c r="V20" s="26">
-        <f t="shared" ref="V20:V32" si="5">T20+U20</f>
+        <f>T20+U20</f>
         <v>50</v>
       </c>
       <c r="W20" s="26"/>
@@ -6053,11 +6067,11 @@
         <v>18</v>
       </c>
       <c r="AH20" s="57">
-        <f t="shared" si="3"/>
+        <f>AE20+AF20+AG20</f>
         <v>23</v>
       </c>
       <c r="AI20" s="57">
-        <f t="shared" ref="AI20:AI30" si="6">AH20+J20</f>
+        <f>AH20+J20</f>
         <v>25</v>
       </c>
       <c r="AJ20" s="4"/>
@@ -6097,107 +6111,108 @@
     </row>
     <row r="21" spans="1:71" s="4" customFormat="1" ht="19.95" customHeight="1">
       <c r="A21" s="54" t="s">
-        <v>225</v>
+        <v>233</v>
       </c>
       <c r="B21" s="32" t="s">
-        <v>109</v>
+        <v>49</v>
       </c>
       <c r="C21" s="36">
-        <v>4.5</v>
+        <v>3.5</v>
       </c>
       <c r="D21" s="37">
-        <v>4.8</v>
+        <v>1.5</v>
       </c>
       <c r="E21" s="38">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F21" s="14">
-        <v>5</v>
-      </c>
-      <c r="G21" s="3" t="s">
-        <v>110</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="G21" s="3"/>
       <c r="H21" s="37">
-        <v>3.5</v>
+        <v>0</v>
       </c>
       <c r="I21" s="15">
-        <f t="shared" si="0"/>
-        <v>4.45</v>
-      </c>
-      <c r="J21" s="15">
+        <f>(C21+D21+F21+H21)/4</f>
+        <v>1.25</v>
+      </c>
+      <c r="J21" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="K21" s="37" t="s">
+        <v>51</v>
+      </c>
+      <c r="L21" s="37" t="s">
+        <v>51</v>
+      </c>
+      <c r="M21" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="N21" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="O21" s="25">
+        <v>31</v>
+      </c>
+      <c r="P21" s="25">
+        <v>27</v>
+      </c>
+      <c r="Q21" s="25">
+        <v>30</v>
+      </c>
+      <c r="R21" s="25">
+        <v>8</v>
+      </c>
+      <c r="S21" s="25">
+        <v>0</v>
+      </c>
+      <c r="T21" s="25">
+        <f>Q21+R21</f>
+        <v>38</v>
+      </c>
+      <c r="U21" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="V21" s="26">
+        <f>T21</f>
+        <v>38</v>
+      </c>
+      <c r="W21" s="26">
+        <v>1</v>
+      </c>
+      <c r="X21" s="57" t="s">
+        <v>54</v>
+      </c>
+      <c r="Y21" s="57">
         <v>2</v>
       </c>
-      <c r="K21" s="37" t="s">
-        <v>111</v>
-      </c>
-      <c r="L21" s="37" t="s">
-        <v>112</v>
-      </c>
-      <c r="M21" s="16">
-        <v>8</v>
-      </c>
-      <c r="N21" s="24" t="s">
-        <v>113</v>
-      </c>
-      <c r="O21" s="25">
-        <v>25</v>
-      </c>
-      <c r="P21" s="25">
-        <v>28</v>
-      </c>
-      <c r="Q21" s="25">
-        <v>36</v>
-      </c>
-      <c r="R21" s="25">
-        <v>4</v>
-      </c>
-      <c r="S21" s="25">
+      <c r="Z21" s="57">
+        <v>22</v>
+      </c>
+      <c r="AA21" s="57">
         <v>1</v>
       </c>
-      <c r="T21" s="25">
-        <f t="shared" si="1"/>
-        <v>40</v>
-      </c>
-      <c r="U21" s="26"/>
-      <c r="V21" s="26">
-        <f t="shared" si="5"/>
-        <v>40</v>
-      </c>
-      <c r="W21" s="26">
-        <v>6</v>
-      </c>
-      <c r="X21" s="57" t="s">
-        <v>36</v>
-      </c>
-      <c r="Y21" s="57">
-        <v>4.5</v>
-      </c>
-      <c r="Z21" s="57">
-        <v>28</v>
-      </c>
-      <c r="AA21" s="57"/>
       <c r="AB21" s="57" t="s">
-        <v>190</v>
+        <v>168</v>
       </c>
       <c r="AC21" s="57" t="s">
-        <v>191</v>
+        <v>238</v>
       </c>
       <c r="AD21" s="58"/>
       <c r="AE21" s="57">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="AF21" s="57">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="AG21" s="57">
         <v>4</v>
       </c>
       <c r="AH21" s="57">
-        <f t="shared" si="3"/>
-        <v>23</v>
+        <f>AE21+AF21+AG21</f>
+        <v>25</v>
       </c>
       <c r="AI21" s="57">
-        <f t="shared" si="6"/>
         <v>25</v>
       </c>
       <c r="BR21" s="3"/>
@@ -6205,7 +6220,7 @@
     </row>
     <row r="22" spans="1:71" s="4" customFormat="1" ht="19.95" customHeight="1">
       <c r="A22" s="54" t="s">
-        <v>226</v>
+        <v>234</v>
       </c>
       <c r="B22" s="40" t="s">
         <v>43</v>
@@ -6229,7 +6244,7 @@
         <v>3.75</v>
       </c>
       <c r="I22" s="42">
-        <f t="shared" si="0"/>
+        <f>(C22+D22+F22+H22)/4</f>
         <v>3.5625</v>
       </c>
       <c r="J22" s="42">
@@ -6263,11 +6278,11 @@
         <v>1</v>
       </c>
       <c r="T22" s="44">
-        <f t="shared" si="1"/>
+        <f>Q22+R22</f>
         <v>41</v>
       </c>
       <c r="V22" s="4">
-        <f t="shared" si="5"/>
+        <f>T22+U22</f>
         <v>41</v>
       </c>
       <c r="W22" s="26">
@@ -6302,11 +6317,11 @@
         <v>12</v>
       </c>
       <c r="AH22" s="57">
-        <f t="shared" si="3"/>
+        <f>AE22+AF22+AG22</f>
         <v>22</v>
       </c>
       <c r="AI22" s="57">
-        <f t="shared" si="6"/>
+        <f>AH22+J22</f>
         <v>22</v>
       </c>
       <c r="BR22" s="3"/>
@@ -6314,7 +6329,7 @@
     </row>
     <row r="23" spans="1:71" s="19" customFormat="1" ht="30.6" customHeight="1">
       <c r="A23" s="54" t="s">
-        <v>227</v>
+        <v>213</v>
       </c>
       <c r="B23" s="40" t="s">
         <v>120</v>
@@ -6338,7 +6353,7 @@
         <v>1.25</v>
       </c>
       <c r="I23" s="42">
-        <f t="shared" si="0"/>
+        <f>(C23+D23+F23+H23)/4</f>
         <v>3.0125000000000002</v>
       </c>
       <c r="J23" s="42">
@@ -6370,12 +6385,12 @@
         <v>1</v>
       </c>
       <c r="T23" s="44">
-        <f t="shared" si="1"/>
+        <f>Q23+R23</f>
         <v>41</v>
       </c>
       <c r="U23" s="4"/>
       <c r="V23" s="4">
-        <f t="shared" si="5"/>
+        <f>T23+U23</f>
         <v>41</v>
       </c>
       <c r="W23" s="26">
@@ -6410,11 +6425,11 @@
         <v>8.5</v>
       </c>
       <c r="AH23" s="57">
-        <f t="shared" si="3"/>
+        <f>AE23+AF23+AG23</f>
         <v>21</v>
       </c>
       <c r="AI23" s="57">
-        <f t="shared" si="6"/>
+        <f>AH23+J23</f>
         <v>21</v>
       </c>
       <c r="AJ23" s="4"/>
@@ -6454,7 +6469,7 @@
     </row>
     <row r="24" spans="1:71" s="4" customFormat="1" ht="19.95" customHeight="1">
       <c r="A24" s="54" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="B24" s="32" t="s">
         <v>96</v>
@@ -6478,7 +6493,7 @@
         <v>3.5</v>
       </c>
       <c r="I24" s="15">
-        <f t="shared" si="0"/>
+        <f>(C24+D24+F24+H24)/4</f>
         <v>3.95</v>
       </c>
       <c r="J24" s="15">
@@ -6512,12 +6527,12 @@
         <v>0</v>
       </c>
       <c r="T24" s="25">
-        <f t="shared" si="1"/>
+        <f>Q24+R24</f>
         <v>8</v>
       </c>
       <c r="U24" s="26"/>
       <c r="V24" s="26">
-        <f t="shared" si="5"/>
+        <f>T24+U24</f>
         <v>8</v>
       </c>
       <c r="W24" s="26"/>
@@ -6550,11 +6565,11 @@
         <v>0</v>
       </c>
       <c r="AH24" s="57">
-        <f t="shared" si="3"/>
+        <f>AE24+AF24+AG24</f>
         <v>17</v>
       </c>
       <c r="AI24" s="57">
-        <f t="shared" si="6"/>
+        <f>AH24+J24</f>
         <v>19</v>
       </c>
       <c r="BR24" s="3"/>
@@ -6562,7 +6577,7 @@
     </row>
     <row r="25" spans="1:71" s="19" customFormat="1" ht="19.95" customHeight="1">
       <c r="A25" s="54" t="s">
-        <v>229</v>
+        <v>215</v>
       </c>
       <c r="B25" s="40" t="s">
         <v>114</v>
@@ -6586,7 +6601,7 @@
         <v>2.25</v>
       </c>
       <c r="I25" s="42">
-        <f t="shared" si="0"/>
+        <f>(C25+D25+F25+H25)/4</f>
         <v>4.2125000000000004</v>
       </c>
       <c r="J25" s="42">
@@ -6618,12 +6633,12 @@
         <v>0</v>
       </c>
       <c r="T25" s="44">
-        <f t="shared" si="1"/>
+        <f>Q25+R25</f>
         <v>44</v>
       </c>
       <c r="U25" s="4"/>
       <c r="V25" s="4">
-        <f t="shared" si="5"/>
+        <f>T25+U25</f>
         <v>44</v>
       </c>
       <c r="W25" s="26">
@@ -6658,11 +6673,11 @@
         <v>5</v>
       </c>
       <c r="AH25" s="57">
-        <f t="shared" si="3"/>
+        <f>AE25+AF25+AG25</f>
         <v>15</v>
       </c>
       <c r="AI25" s="57">
-        <f t="shared" si="6"/>
+        <f>AH25+J25</f>
         <v>17</v>
       </c>
       <c r="AJ25" s="4"/>
@@ -6702,7 +6717,7 @@
     </row>
     <row r="26" spans="1:71" s="4" customFormat="1" ht="19.95" customHeight="1">
       <c r="A26" s="54" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="B26" s="32" t="s">
         <v>74</v>
@@ -6726,7 +6741,7 @@
         <v>2.5</v>
       </c>
       <c r="I26" s="15">
-        <f t="shared" si="0"/>
+        <f>(C26+D26+F26+H26)/4</f>
         <v>3.625</v>
       </c>
       <c r="J26" s="15">
@@ -6760,12 +6775,12 @@
         <v>0</v>
       </c>
       <c r="T26" s="25">
-        <f t="shared" si="1"/>
+        <f>Q26+R26</f>
         <v>41</v>
       </c>
       <c r="U26" s="26"/>
       <c r="V26" s="26">
-        <f t="shared" si="5"/>
+        <f>T26+U26</f>
         <v>41</v>
       </c>
       <c r="W26" s="26">
@@ -6802,11 +6817,11 @@
         <v>6</v>
       </c>
       <c r="AH26" s="57">
-        <f t="shared" si="3"/>
+        <f>AE26+AF26+AG26</f>
         <v>16</v>
       </c>
       <c r="AI26" s="57">
-        <f t="shared" si="6"/>
+        <f>AH26+J26</f>
         <v>16</v>
       </c>
       <c r="BR26" s="3"/>
@@ -6814,7 +6829,7 @@
     </row>
     <row r="27" spans="1:71" s="23" customFormat="1" ht="19.95" customHeight="1">
       <c r="A27" s="54" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="B27" s="32" t="s">
         <v>82</v>
@@ -6838,7 +6853,7 @@
         <v>2.5</v>
       </c>
       <c r="I27" s="15">
-        <f t="shared" si="0"/>
+        <f>(C27+D27+F27+H27)/4</f>
         <v>4.375</v>
       </c>
       <c r="J27" s="15">
@@ -6872,20 +6887,20 @@
         <v>0</v>
       </c>
       <c r="T27" s="25">
-        <f t="shared" si="1"/>
+        <f>Q27+R27</f>
         <v>44</v>
       </c>
       <c r="U27" s="26">
         <v>1</v>
       </c>
       <c r="V27" s="26">
-        <f t="shared" si="5"/>
+        <f>T27+U27</f>
         <v>45</v>
       </c>
       <c r="W27" s="26" t="s">
         <v>86</v>
       </c>
-      <c r="X27" s="68" t="s">
+      <c r="X27" s="62" t="s">
         <v>40</v>
       </c>
       <c r="Y27" s="57">
@@ -6914,11 +6929,11 @@
         <v>0</v>
       </c>
       <c r="AH27" s="57">
-        <f t="shared" si="3"/>
+        <f>AE27+AF27+AG27</f>
         <v>12</v>
       </c>
       <c r="AI27" s="57">
-        <f t="shared" si="6"/>
+        <f>AH27+J27</f>
         <v>12</v>
       </c>
       <c r="BR27" s="22"/>
@@ -6926,111 +6941,105 @@
     </row>
     <row r="28" spans="1:71" s="4" customFormat="1" ht="19.95" customHeight="1">
       <c r="A28" s="54" t="s">
-        <v>232</v>
+        <v>208</v>
       </c>
       <c r="B28" s="32" t="s">
-        <v>126</v>
+        <v>137</v>
       </c>
       <c r="C28" s="11">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D28" s="12">
-        <v>5</v>
+        <v>3.4</v>
       </c>
       <c r="E28" s="13">
+        <v>3.75</v>
+      </c>
+      <c r="F28" s="14">
+        <v>5</v>
+      </c>
+      <c r="G28" s="3"/>
+      <c r="H28" s="12">
+        <v>2.5</v>
+      </c>
+      <c r="I28" s="15">
+        <f>(C28+D28+F28+H28)/4</f>
+        <v>3.7250000000000001</v>
+      </c>
+      <c r="J28" s="15">
         <v>2</v>
       </c>
-      <c r="F28" s="14">
-        <v>5</v>
-      </c>
-      <c r="G28" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="H28" s="12">
-        <v>0</v>
-      </c>
-      <c r="I28" s="15">
-        <f t="shared" si="0"/>
-        <v>3.75</v>
-      </c>
-      <c r="J28" s="15">
-        <v>0</v>
-      </c>
-      <c r="K28" s="12" t="s">
-        <v>90</v>
-      </c>
+      <c r="K28" s="12"/>
       <c r="L28" s="12" t="s">
-        <v>91</v>
+        <v>138</v>
       </c>
       <c r="M28" s="16">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N28" s="24" t="s">
-        <v>128</v>
+        <v>139</v>
       </c>
       <c r="O28" s="25">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="P28" s="25">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="Q28" s="25">
-        <v>7</v>
+        <v>36</v>
       </c>
       <c r="R28" s="25">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="S28" s="25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T28" s="25">
-        <f t="shared" si="1"/>
-        <v>15</v>
+        <f>Q28+R28</f>
+        <v>42</v>
       </c>
       <c r="U28" s="26"/>
       <c r="V28" s="26">
-        <f t="shared" si="5"/>
-        <v>15</v>
-      </c>
-      <c r="W28" s="56" t="s">
-        <v>129</v>
-      </c>
-      <c r="X28" s="59" t="s">
+        <f>T28+U28</f>
         <v>42</v>
       </c>
-      <c r="Y28" s="59">
-        <v>2.5</v>
-      </c>
-      <c r="Z28" s="59">
-        <v>25</v>
-      </c>
-      <c r="AA28" s="59" t="s">
-        <v>195</v>
-      </c>
-      <c r="AB28" s="59" t="s">
-        <v>197</v>
-      </c>
-      <c r="AC28" s="59" t="s">
+      <c r="W28" s="26">
+        <v>11</v>
+      </c>
+      <c r="X28" s="57" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y28" s="57">
+        <v>4</v>
+      </c>
+      <c r="Z28" s="57">
+        <v>21</v>
+      </c>
+      <c r="AA28" s="57" t="s">
+        <v>198</v>
+      </c>
+      <c r="AB28" s="57" t="s">
+        <v>199</v>
+      </c>
+      <c r="AC28" s="57" t="s">
         <v>87</v>
       </c>
-      <c r="AD28" s="60" t="s">
-        <v>196</v>
-      </c>
-      <c r="AE28" s="59">
+      <c r="AD28" s="58"/>
+      <c r="AE28" s="57">
+        <v>5</v>
+      </c>
+      <c r="AF28" s="57">
         <v>3</v>
       </c>
-      <c r="AF28" s="59">
-        <v>7</v>
-      </c>
-      <c r="AG28" s="59">
+      <c r="AG28" s="57">
         <v>0</v>
       </c>
-      <c r="AH28" s="59">
-        <f t="shared" si="3"/>
-        <v>10</v>
-      </c>
-      <c r="AI28" s="59">
-        <f t="shared" si="6"/>
+      <c r="AH28" s="57">
+        <f>AE28+AF28+AG28</f>
+        <v>8</v>
+      </c>
+      <c r="AI28" s="57">
+        <f>AH28+J28</f>
         <v>10</v>
       </c>
       <c r="BR28" s="3"/>
@@ -7038,105 +7047,111 @@
     </row>
     <row r="29" spans="1:71" s="4" customFormat="1" ht="19.95" customHeight="1">
       <c r="A29" s="54" t="s">
-        <v>233</v>
+        <v>211</v>
       </c>
       <c r="B29" s="32" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="C29" s="11">
+        <v>5</v>
+      </c>
+      <c r="D29" s="12">
+        <v>5</v>
+      </c>
+      <c r="E29" s="13">
+        <v>2</v>
+      </c>
+      <c r="F29" s="14">
+        <v>5</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="H29" s="12">
+        <v>0</v>
+      </c>
+      <c r="I29" s="15">
+        <f>(C29+D29+F29+H29)/4</f>
+        <v>3.75</v>
+      </c>
+      <c r="J29" s="15">
+        <v>0</v>
+      </c>
+      <c r="K29" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="L29" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="M29" s="16">
         <v>4</v>
       </c>
-      <c r="D29" s="12">
-        <v>3.4</v>
-      </c>
-      <c r="E29" s="13">
-        <v>3.75</v>
-      </c>
-      <c r="F29" s="14">
-        <v>5</v>
-      </c>
-      <c r="G29" s="3"/>
-      <c r="H29" s="12">
-        <v>2.5</v>
-      </c>
-      <c r="I29" s="15">
-        <f t="shared" si="0"/>
-        <v>3.7250000000000001</v>
-      </c>
-      <c r="J29" s="15">
-        <v>2</v>
-      </c>
-      <c r="K29" s="12"/>
-      <c r="L29" s="12" t="s">
-        <v>138</v>
-      </c>
-      <c r="M29" s="16">
-        <v>3</v>
-      </c>
       <c r="N29" s="24" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
       <c r="O29" s="25">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="P29" s="25">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="Q29" s="25">
-        <v>36</v>
+        <v>7</v>
       </c>
       <c r="R29" s="25">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="S29" s="25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T29" s="25">
-        <f t="shared" si="1"/>
-        <v>42</v>
+        <f>Q29+R29</f>
+        <v>15</v>
       </c>
       <c r="U29" s="26"/>
       <c r="V29" s="26">
-        <f t="shared" si="5"/>
+        <f>T29+U29</f>
+        <v>15</v>
+      </c>
+      <c r="W29" s="56" t="s">
+        <v>129</v>
+      </c>
+      <c r="X29" s="59" t="s">
         <v>42</v>
       </c>
-      <c r="W29" s="26">
-        <v>11</v>
-      </c>
-      <c r="X29" s="57" t="s">
-        <v>36</v>
-      </c>
-      <c r="Y29" s="57">
-        <v>4</v>
-      </c>
-      <c r="Z29" s="57">
-        <v>21</v>
-      </c>
-      <c r="AA29" s="57" t="s">
-        <v>198</v>
-      </c>
-      <c r="AB29" s="57" t="s">
-        <v>199</v>
-      </c>
-      <c r="AC29" s="57" t="s">
+      <c r="Y29" s="59">
+        <v>2.5</v>
+      </c>
+      <c r="Z29" s="59">
+        <v>25</v>
+      </c>
+      <c r="AA29" s="59" t="s">
+        <v>195</v>
+      </c>
+      <c r="AB29" s="59" t="s">
+        <v>197</v>
+      </c>
+      <c r="AC29" s="59" t="s">
         <v>87</v>
       </c>
-      <c r="AD29" s="58"/>
-      <c r="AE29" s="57">
-        <v>5</v>
-      </c>
-      <c r="AF29" s="57">
+      <c r="AD29" s="60" t="s">
+        <v>196</v>
+      </c>
+      <c r="AE29" s="59">
         <v>3</v>
       </c>
-      <c r="AG29" s="57">
+      <c r="AF29" s="59">
+        <v>7</v>
+      </c>
+      <c r="AG29" s="59">
         <v>0</v>
       </c>
-      <c r="AH29" s="57">
-        <f t="shared" si="3"/>
-        <v>8</v>
-      </c>
-      <c r="AI29" s="57">
-        <f t="shared" si="6"/>
+      <c r="AH29" s="59">
+        <f>AE29+AF29+AG29</f>
+        <v>10</v>
+      </c>
+      <c r="AI29" s="59">
+        <f>AH29+J29</f>
         <v>10</v>
       </c>
       <c r="BR29" s="3"/>
@@ -7144,7 +7159,7 @@
     </row>
     <row r="30" spans="1:71" s="4" customFormat="1" ht="19.95" customHeight="1">
       <c r="A30" s="54" t="s">
-        <v>234</v>
+        <v>222</v>
       </c>
       <c r="B30" s="32" t="s">
         <v>93</v>
@@ -7168,7 +7183,7 @@
         <v>4</v>
       </c>
       <c r="I30" s="15">
-        <f t="shared" si="0"/>
+        <f>(C30+D30+F30+H30)/4</f>
         <v>4.3</v>
       </c>
       <c r="J30" s="15">
@@ -7202,12 +7217,12 @@
         <v>2</v>
       </c>
       <c r="T30" s="25">
-        <f t="shared" si="1"/>
+        <f>Q30+R30</f>
         <v>40</v>
       </c>
       <c r="U30" s="26"/>
       <c r="V30" s="26">
-        <f t="shared" si="5"/>
+        <f>T30+U30</f>
         <v>40</v>
       </c>
       <c r="W30" s="26">
@@ -7242,11 +7257,11 @@
         <v>0</v>
       </c>
       <c r="AH30" s="57">
-        <f t="shared" si="3"/>
+        <f>AE30+AF30+AG30</f>
         <v>2</v>
       </c>
       <c r="AI30" s="57">
-        <f t="shared" si="6"/>
+        <f>AH30+J30</f>
         <v>2</v>
       </c>
       <c r="BR30" s="3"/>
@@ -7254,98 +7269,105 @@
     </row>
     <row r="31" spans="1:71" s="4" customFormat="1" ht="19.95" customHeight="1">
       <c r="A31" s="54" t="s">
-        <v>235</v>
-      </c>
-      <c r="B31" s="40" t="s">
-        <v>103</v>
-      </c>
-      <c r="C31" s="45">
-        <v>5</v>
-      </c>
-      <c r="D31" s="46">
-        <v>5</v>
-      </c>
-      <c r="E31" s="47">
-        <v>4.9000000000000004</v>
-      </c>
-      <c r="F31" s="41">
-        <v>5</v>
-      </c>
-      <c r="G31" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="H31" s="46">
+        <v>232</v>
+      </c>
+      <c r="B31" s="63" t="s">
+        <v>55</v>
+      </c>
+      <c r="C31" s="66">
+        <v>3</v>
+      </c>
+      <c r="D31" s="68">
         <v>0</v>
       </c>
-      <c r="I31" s="42">
-        <f t="shared" si="0"/>
+      <c r="E31" s="70">
+        <v>2.5</v>
+      </c>
+      <c r="F31" s="49">
+        <v>2.5</v>
+      </c>
+      <c r="G31" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="H31" s="71">
         <v>3.75</v>
       </c>
-      <c r="J31" s="42" t="s">
+      <c r="I31" s="72">
+        <f>(C31+D31+F31+H31)/4</f>
+        <v>2.3125</v>
+      </c>
+      <c r="J31" s="72" t="s">
         <v>50</v>
       </c>
-      <c r="K31" s="46" t="s">
-        <v>94</v>
-      </c>
-      <c r="L31" s="46" t="s">
-        <v>34</v>
-      </c>
-      <c r="M31" s="43">
-        <v>6</v>
-      </c>
-      <c r="N31" s="41" t="s">
-        <v>104</v>
-      </c>
-      <c r="O31" s="44">
-        <v>12</v>
-      </c>
-      <c r="P31" s="44">
+      <c r="K31" s="71" t="s">
+        <v>57</v>
+      </c>
+      <c r="L31" s="71" t="s">
+        <v>58</v>
+      </c>
+      <c r="M31" s="50" t="s">
+        <v>40</v>
+      </c>
+      <c r="N31" s="49" t="s">
+        <v>59</v>
+      </c>
+      <c r="O31" s="51">
+        <v>24</v>
+      </c>
+      <c r="P31" s="51">
         <v>9</v>
       </c>
-      <c r="Q31" s="44">
-        <v>34</v>
-      </c>
-      <c r="R31" s="44">
+      <c r="Q31" s="51">
+        <v>19</v>
+      </c>
+      <c r="R31" s="51">
+        <v>0</v>
+      </c>
+      <c r="S31" s="51">
         <v>2</v>
       </c>
-      <c r="S31" s="44">
+      <c r="T31" s="51">
+        <f>Q31+R31</f>
+        <v>19</v>
+      </c>
+      <c r="U31" s="23"/>
+      <c r="V31" s="4">
+        <f>T31+U31</f>
+        <v>19</v>
+      </c>
+      <c r="W31" s="26">
+        <v>4</v>
+      </c>
+      <c r="X31" s="57" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y31" s="57">
+        <v>2</v>
+      </c>
+      <c r="Z31" s="57">
+        <v>26</v>
+      </c>
+      <c r="AA31" s="62" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB31" s="62" t="s">
+        <v>40</v>
+      </c>
+      <c r="AC31" s="62" t="s">
+        <v>40</v>
+      </c>
+      <c r="AD31" s="58"/>
+      <c r="AE31" s="57">
         <v>0</v>
       </c>
-      <c r="T31" s="44">
-        <f t="shared" si="1"/>
-        <v>36</v>
-      </c>
-      <c r="V31" s="4">
-        <f t="shared" si="5"/>
-        <v>36</v>
-      </c>
-      <c r="W31" s="26">
-        <v>8</v>
-      </c>
-      <c r="X31" s="57" t="s">
-        <v>42</v>
-      </c>
-      <c r="Y31" s="57">
+      <c r="AF31" s="57">
         <v>0</v>
       </c>
-      <c r="Z31" s="57">
+      <c r="AG31" s="57">
         <v>0</v>
       </c>
-      <c r="AA31" s="68" t="s">
-        <v>40</v>
-      </c>
-      <c r="AB31" s="68" t="s">
-        <v>40</v>
-      </c>
-      <c r="AC31" s="68" t="s">
-        <v>40</v>
-      </c>
-      <c r="AD31" s="58"/>
-      <c r="AE31" s="57"/>
-      <c r="AF31" s="57"/>
-      <c r="AG31" s="57"/>
       <c r="AH31" s="57">
-        <f t="shared" si="3"/>
+        <f>AE31+AF31+AG31</f>
         <v>0</v>
       </c>
       <c r="AI31" s="57">
@@ -7354,107 +7376,100 @@
       <c r="BR31" s="3"/>
       <c r="BS31" s="3"/>
     </row>
-    <row r="32" spans="1:71" ht="69">
+    <row r="32" spans="1:71" ht="82.8">
       <c r="A32" s="54" t="s">
-        <v>236</v>
-      </c>
-      <c r="B32" s="62" t="s">
-        <v>55</v>
-      </c>
-      <c r="C32" s="63">
-        <v>3</v>
-      </c>
-      <c r="D32" s="64">
+        <v>219</v>
+      </c>
+      <c r="B32" s="64" t="s">
+        <v>103</v>
+      </c>
+      <c r="C32" s="65">
+        <v>5</v>
+      </c>
+      <c r="D32" s="67">
+        <v>5</v>
+      </c>
+      <c r="E32" s="69">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="F32" s="41">
+        <v>5</v>
+      </c>
+      <c r="G32" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="H32" s="67">
         <v>0</v>
       </c>
-      <c r="E32" s="65">
-        <v>2.5</v>
-      </c>
-      <c r="F32" s="49">
-        <v>2.5</v>
-      </c>
-      <c r="G32" s="23" t="s">
-        <v>56</v>
-      </c>
-      <c r="H32" s="66">
+      <c r="I32" s="73">
+        <f>(C32+D32+F32+H32)/4</f>
         <v>3.75</v>
       </c>
-      <c r="I32" s="67">
-        <f t="shared" si="0"/>
-        <v>2.3125</v>
-      </c>
-      <c r="J32" s="67" t="s">
+      <c r="J32" s="73" t="s">
         <v>50</v>
       </c>
-      <c r="K32" s="66" t="s">
-        <v>57</v>
-      </c>
-      <c r="L32" s="66" t="s">
-        <v>58</v>
-      </c>
-      <c r="M32" s="50" t="s">
+      <c r="K32" s="67" t="s">
+        <v>94</v>
+      </c>
+      <c r="L32" s="67" t="s">
+        <v>34</v>
+      </c>
+      <c r="M32" s="43">
+        <v>6</v>
+      </c>
+      <c r="N32" s="41" t="s">
+        <v>104</v>
+      </c>
+      <c r="O32" s="44">
+        <v>12</v>
+      </c>
+      <c r="P32" s="44">
+        <v>9</v>
+      </c>
+      <c r="Q32" s="44">
+        <v>34</v>
+      </c>
+      <c r="R32" s="44">
+        <v>2</v>
+      </c>
+      <c r="S32" s="44">
+        <v>0</v>
+      </c>
+      <c r="T32" s="44">
+        <f>Q32+R32</f>
+        <v>36</v>
+      </c>
+      <c r="V32" s="4">
+        <f>T32+U32</f>
+        <v>36</v>
+      </c>
+      <c r="W32" s="26">
+        <v>8</v>
+      </c>
+      <c r="X32" s="57" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y32" s="57">
+        <v>0</v>
+      </c>
+      <c r="Z32" s="57">
+        <v>0</v>
+      </c>
+      <c r="AA32" s="62" t="s">
         <v>40</v>
       </c>
-      <c r="N32" s="49" t="s">
-        <v>59</v>
-      </c>
-      <c r="O32" s="51">
-        <v>24</v>
-      </c>
-      <c r="P32" s="51">
-        <v>9</v>
-      </c>
-      <c r="Q32" s="51">
-        <v>19</v>
-      </c>
-      <c r="R32" s="51">
-        <v>0</v>
-      </c>
-      <c r="S32" s="51">
-        <v>2</v>
-      </c>
-      <c r="T32" s="51">
-        <f t="shared" si="1"/>
-        <v>19</v>
-      </c>
-      <c r="U32" s="23"/>
-      <c r="V32" s="4">
-        <f t="shared" si="5"/>
-        <v>19</v>
-      </c>
-      <c r="W32" s="26">
-        <v>4</v>
-      </c>
-      <c r="X32" s="57" t="s">
-        <v>36</v>
-      </c>
-      <c r="Y32" s="57">
-        <v>2</v>
-      </c>
-      <c r="Z32" s="57">
-        <v>26</v>
-      </c>
-      <c r="AA32" s="68" t="s">
+      <c r="AB32" s="62" t="s">
         <v>40</v>
       </c>
-      <c r="AB32" s="68" t="s">
+      <c r="AC32" s="62" t="s">
         <v>40</v>
       </c>
-      <c r="AC32" s="68" t="s">
-        <v>40</v>
-      </c>
       <c r="AD32" s="58"/>
-      <c r="AE32" s="57">
-        <v>0</v>
-      </c>
-      <c r="AF32" s="57">
-        <v>0</v>
-      </c>
-      <c r="AG32" s="57">
-        <v>0</v>
-      </c>
+      <c r="AE32" s="57"/>
+      <c r="AF32" s="57"/>
+      <c r="AG32" s="57"/>
       <c r="AH32" s="57">
-        <f t="shared" si="3"/>
+        <f>AE32+AF32+AG32</f>
         <v>0</v>
       </c>
       <c r="AI32" s="57">
@@ -7462,9 +7477,9 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="zy8rQGEROMnO9QyKyYo7gwTijyh1HBc7g97RoJOvqp6NRuafTbZn5VmxQL3sMOW2PN8jVSjIG6BSQtgkjkaWUA==" saltValue="1xIrSY0tvN4I2Rv6nopzsw==" spinCount="100000" sheet="1" sort="0" autoFilter="0"/>
-  <autoFilter ref="B2:AI32" xr:uid="{97AC2FA6-0FD9-4A0A-8A86-68E6A69CAF3C}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:AI32">
+  <sheetProtection algorithmName="SHA-512" hashValue="XBzAiY1tCRBGz9ZQ/CZi7E6IuCAVIdb2fRretQmZmX+8T+FFiURf2bbGaEUp0RgSIkw1bj1mANOFw0F5fV0EkA==" saltValue="AZtTh5YCtgiF+lFanP1C6Q==" spinCount="100000" sheet="1" objects="1" scenarios="1" sort="0" autoFilter="0"/>
+  <autoFilter ref="A2:AI32" xr:uid="{DB4A43FE-0C9C-4BEF-8605-3D126051B053}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:AI32">
       <sortCondition descending="1" ref="AI2:AI32"/>
     </sortState>
   </autoFilter>

</xml_diff>